<commit_message>
pushing final changes to machine learning model and excel file
</commit_message>
<xml_diff>
--- a/Model_Building_Optimization/ML_ModelSummary.xlsx
+++ b/Model_Building_Optimization/ML_ModelSummary.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/santiagonavarroroby1/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/santiagonavarroroby1/Desktop/GWBootCamp/Projects/Project4/Stroke_ML/Model_Building_Optimization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D9DF9DF-481F-9440-8EBF-D7547AA5DF16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D615685C-39BF-E04C-A9FD-250614169C1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33500" yWindow="1940" windowWidth="34280" windowHeight="17440" xr2:uid="{BDD10E18-A5C1-944A-9779-923E8715CA5A}"/>
   </bookViews>
@@ -206,7 +206,7 @@
     <t>• n_neighbors = 3</t>
   </si>
   <si>
-    <t>•n_neighbors = 4</t>
+    <t>•n_neighbors = 5</t>
   </si>
 </sst>
 </file>
@@ -898,22 +898,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>215900</xdr:colOff>
+      <xdr:colOff>444500</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>330200</xdr:rowOff>
+      <xdr:rowOff>317500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>6096000</xdr:colOff>
+      <xdr:colOff>5889384</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>2209800</xdr:rowOff>
+      <xdr:rowOff>2159000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="19" name="Picture 18">
+        <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{17120478-D1C3-7211-8F7F-7A91EC3FAFC7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F2B40DC9-442D-CA4B-F157-571686311FF0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -921,22 +921,15 @@
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:srcRect l="10461" t="42244" r="32749"/>
+        <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10858500" y="20662900"/>
-          <a:ext cx="5880100" cy="1879600"/>
+          <a:off x="11087100" y="20650200"/>
+          <a:ext cx="5444884" cy="1841500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1247,8 +1240,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{258A020A-A0A6-AB4A-8412-4546A2B710E4}">
   <dimension ref="C3:H16"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E11" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1441,7 +1434,7 @@
         <v>13</v>
       </c>
       <c r="F16" s="19">
-        <v>0.95</v>
+        <v>0.93</v>
       </c>
       <c r="G16" s="5"/>
       <c r="H16" s="5" t="s">

</xml_diff>